<commit_message>
Model. node_balance_penalty_p_up, node_balance_penalty_p_down, node_balance_penalty_q_up and node_balance_penalty_q_down added.
</commit_message>
<xml_diff>
--- a/data/HR3/Market Data/HR3_market_data_2020.xlsx
+++ b/data/HR3/Market Data/HR3_market_data_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resource-planning-no_esso-v2\data\HR3\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7836C11A-443C-415B-BD45-0F8C91BB8AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6549FFA6-67DD-46AA-BD97-81B8C8937744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3540" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9720" yWindow="3180" windowWidth="21600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -859,7 +859,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,11 +872,10 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1">
         <f>1/3</f>

</xml_diff>